<commit_message>
AJout Schéma élec + cablage driver Pas à Pas
</commit_message>
<xml_diff>
--- a/Liste composant turtlebot carte.xlsx
+++ b/Liste composant turtlebot carte.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Nom</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>http://fr.rs-online.com/web/p/led/4663548/</t>
+  </si>
+  <si>
+    <t>74hc595</t>
   </si>
 </sst>
 </file>
@@ -436,7 +439,7 @@
   <dimension ref="C1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,6 +561,14 @@
         <v>19</v>
       </c>
     </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+    </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
MAJ pdf schéma élec
</commit_message>
<xml_diff>
--- a/Liste composant turtlebot carte.xlsx
+++ b/Liste composant turtlebot carte.xlsx
@@ -439,7 +439,7 @@
   <dimension ref="C1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +544,7 @@
         <v>13</v>
       </c>
       <c r="F8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="3:16" x14ac:dyDescent="0.25">

</xml_diff>